<commit_message>
data variable name change
</commit_message>
<xml_diff>
--- a/data/candidates.xlsx
+++ b/data/candidates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\OneDrive\Dokumente\Research\implicitdiscrimination\implicitdiscrimination\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE59EF33-5E97-4DA4-A5E1-6375311A8A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F71BBD-E7A9-4092-B926-E9E7928F15A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="108" windowWidth="20616" windowHeight="12276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
   <si>
-    <t>participant.time_started</t>
-  </si>
-  <si>
     <t>Mathematik</t>
   </si>
   <si>
@@ -707,6 +704,9 @@
   </si>
   <si>
     <t>payofftotal</t>
+  </si>
+  <si>
+    <t>time_started</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,40 +1099,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
         <v>222</v>
       </c>
-      <c r="B1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>223</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>224</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>225</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>226</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>227</v>
-      </c>
-      <c r="L1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1140,10 +1140,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -1178,10 +1178,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1199,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J3">
         <v>50</v>
@@ -1216,10 +1216,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>60</v>
@@ -1254,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5">
         <v>51</v>
@@ -1292,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1313,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6">
         <v>75</v>
@@ -1330,10 +1330,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7">
         <v>50</v>
@@ -1368,10 +1368,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -1389,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8">
         <v>100</v>
@@ -1406,10 +1406,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
       </c>
       <c r="D9">
         <v>9</v>
@@ -1427,7 +1427,7 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9">
         <v>70</v>
@@ -1444,10 +1444,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
       <c r="D10">
         <v>11</v>
@@ -1465,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10">
         <v>65</v>
@@ -1482,10 +1482,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11">
         <v>50</v>
@@ -1520,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1541,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <v>50</v>
@@ -1558,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -1579,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13">
         <v>50</v>
@@ -1596,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1617,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14">
         <v>50</v>
@@ -1634,10 +1634,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15">
         <v>40</v>
@@ -1672,10 +1672,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J16">
         <v>75</v>
@@ -1710,10 +1710,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -1731,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17">
         <v>50</v>
@@ -1748,10 +1748,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1769,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18">
         <v>60</v>
@@ -1786,10 +1786,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
         <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -1807,7 +1807,7 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J19">
         <v>60</v>
@@ -1824,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
         <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1845,7 +1845,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J20">
         <v>50</v>
@@ -1862,10 +1862,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -1883,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J21">
         <v>60</v>
@@ -1900,10 +1900,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
       </c>
       <c r="D22">
         <v>13</v>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J22">
         <v>55</v>
@@ -1938,10 +1938,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
       </c>
       <c r="D23">
         <v>13</v>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23">
         <v>10</v>
@@ -1976,10 +1976,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1997,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24">
         <v>64</v>
@@ -2014,10 +2014,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
       </c>
       <c r="D25">
         <v>9</v>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J25">
         <v>63</v>
@@ -2052,10 +2052,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
         <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -2073,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J26">
         <v>40</v>
@@ -2090,10 +2090,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -2111,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J27">
         <v>60</v>
@@ -2128,10 +2128,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
       </c>
       <c r="D28">
         <v>12</v>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J28">
         <v>60</v>
@@ -2166,10 +2166,10 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
         <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -2187,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J29">
         <v>60</v>
@@ -2204,10 +2204,10 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" t="s">
         <v>83</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
       </c>
       <c r="D30">
         <v>9</v>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J30">
         <v>60</v>
@@ -2242,10 +2242,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
         <v>86</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
       </c>
       <c r="D31">
         <v>7</v>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J31">
         <v>75</v>
@@ -2280,10 +2280,10 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
       </c>
       <c r="D32">
         <v>15</v>
@@ -2301,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J32">
         <v>25</v>
@@ -2318,10 +2318,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
         <v>92</v>
-      </c>
-      <c r="C33" t="s">
-        <v>93</v>
       </c>
       <c r="D33">
         <v>9</v>
@@ -2339,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J33">
         <v>40</v>
@@ -2356,10 +2356,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>95</v>
       </c>
       <c r="D34">
         <v>13</v>
@@ -2377,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J34">
         <v>40</v>
@@ -2394,10 +2394,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
         <v>97</v>
-      </c>
-      <c r="C35" t="s">
-        <v>98</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -2415,7 +2415,7 @@
         <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J35">
         <v>40</v>
@@ -2432,10 +2432,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
         <v>100</v>
-      </c>
-      <c r="C36" t="s">
-        <v>101</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -2453,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J36">
         <v>80</v>
@@ -2470,10 +2470,10 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
       </c>
       <c r="D37">
         <v>7</v>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <v>50</v>
@@ -2508,10 +2508,10 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
         <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>106</v>
       </c>
       <c r="D38">
         <v>18</v>
@@ -2529,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J38">
         <v>80</v>
@@ -2546,10 +2546,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
         <v>107</v>
-      </c>
-      <c r="C39" t="s">
-        <v>108</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -2567,7 +2567,7 @@
         <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J39">
         <v>50</v>
@@ -2584,10 +2584,10 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
         <v>110</v>
-      </c>
-      <c r="C40" t="s">
-        <v>111</v>
       </c>
       <c r="D40">
         <v>10</v>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J40">
         <v>50</v>
@@ -2622,10 +2622,10 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
         <v>113</v>
-      </c>
-      <c r="C41" t="s">
-        <v>114</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -2643,7 +2643,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J41">
         <v>100</v>
@@ -2660,10 +2660,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" t="s">
         <v>116</v>
-      </c>
-      <c r="C42" t="s">
-        <v>117</v>
       </c>
       <c r="D42">
         <v>12</v>
@@ -2681,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J42">
         <v>50</v>
@@ -2698,10 +2698,10 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s">
         <v>118</v>
-      </c>
-      <c r="C43" t="s">
-        <v>119</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J43">
         <v>50</v>
@@ -2736,10 +2736,10 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" t="s">
-        <v>121</v>
       </c>
       <c r="D44">
         <v>15</v>
@@ -2757,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J44">
         <v>60</v>
@@ -2774,10 +2774,10 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" t="s">
         <v>123</v>
-      </c>
-      <c r="C45" t="s">
-        <v>124</v>
       </c>
       <c r="D45">
         <v>13</v>
@@ -2795,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J45">
         <v>70</v>
@@ -2812,10 +2812,10 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" t="s">
         <v>125</v>
-      </c>
-      <c r="C46" t="s">
-        <v>126</v>
       </c>
       <c r="D46">
         <v>7</v>
@@ -2833,7 +2833,7 @@
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J46">
         <v>30</v>
@@ -2850,10 +2850,10 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" t="s">
         <v>127</v>
-      </c>
-      <c r="C47" t="s">
-        <v>128</v>
       </c>
       <c r="D47">
         <v>5</v>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J47">
         <v>30</v>
@@ -2888,10 +2888,10 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
         <v>130</v>
-      </c>
-      <c r="C48" t="s">
-        <v>131</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J48">
         <v>70</v>
@@ -2926,10 +2926,10 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="s">
         <v>133</v>
-      </c>
-      <c r="C49" t="s">
-        <v>134</v>
       </c>
       <c r="D49">
         <v>4</v>
@@ -2947,7 +2947,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J49">
         <v>40</v>
@@ -2964,10 +2964,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" t="s">
         <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>137</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -2985,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J50">
         <v>20</v>
@@ -3002,10 +3002,10 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
         <v>138</v>
-      </c>
-      <c r="C51" t="s">
-        <v>139</v>
       </c>
       <c r="D51">
         <v>4</v>
@@ -3023,7 +3023,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J51">
         <v>50</v>
@@ -3040,10 +3040,10 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
         <v>140</v>
-      </c>
-      <c r="C52" t="s">
-        <v>141</v>
       </c>
       <c r="D52">
         <v>13</v>
@@ -3061,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="I52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J52">
         <v>50</v>
@@ -3078,10 +3078,10 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" t="s">
         <v>143</v>
-      </c>
-      <c r="C53" t="s">
-        <v>144</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -3099,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="I53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J53">
         <v>40</v>
@@ -3116,10 +3116,10 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" t="s">
         <v>146</v>
-      </c>
-      <c r="C54" t="s">
-        <v>147</v>
       </c>
       <c r="D54">
         <v>6</v>
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J54">
         <v>50</v>
@@ -3154,10 +3154,10 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" t="s">
         <v>148</v>
-      </c>
-      <c r="C55" t="s">
-        <v>149</v>
       </c>
       <c r="D55">
         <v>11</v>
@@ -3175,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="I55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J55">
         <v>75</v>
@@ -3192,10 +3192,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" t="s">
         <v>151</v>
-      </c>
-      <c r="C56" t="s">
-        <v>152</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -3213,7 +3213,7 @@
         <v>2</v>
       </c>
       <c r="I56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J56">
         <v>50</v>
@@ -3230,10 +3230,10 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s">
         <v>153</v>
-      </c>
-      <c r="C57" t="s">
-        <v>154</v>
       </c>
       <c r="D57">
         <v>10</v>
@@ -3251,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J57">
         <v>60</v>
@@ -3268,10 +3268,10 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58" t="s">
         <v>156</v>
-      </c>
-      <c r="C58" t="s">
-        <v>157</v>
       </c>
       <c r="D58">
         <v>14</v>
@@ -3289,7 +3289,7 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J58">
         <v>60</v>
@@ -3306,10 +3306,10 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D59">
         <v>6</v>
@@ -3327,7 +3327,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J59">
         <v>60</v>
@@ -3344,10 +3344,10 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" t="s">
         <v>161</v>
-      </c>
-      <c r="C60" t="s">
-        <v>162</v>
       </c>
       <c r="D60">
         <v>8</v>
@@ -3365,7 +3365,7 @@
         <v>2</v>
       </c>
       <c r="I60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J60">
         <v>50</v>
@@ -3382,10 +3382,10 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" t="s">
         <v>163</v>
-      </c>
-      <c r="C61" t="s">
-        <v>164</v>
       </c>
       <c r="D61">
         <v>5</v>
@@ -3403,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J61">
         <v>40</v>
@@ -3420,10 +3420,10 @@
         <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D62" s="2">
         <v>8</v>
@@ -3441,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J62" s="2">
         <v>50</v>
@@ -3465,10 +3465,10 @@
         <v>4</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D63" s="2">
         <v>13</v>
@@ -3486,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J63" s="2">
         <v>60</v>
@@ -3510,10 +3510,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="D64" s="2">
         <v>9</v>
@@ -3531,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J64" s="2">
         <v>60</v>
@@ -3555,10 +3555,10 @@
         <v>4</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="D65" s="2">
         <v>7</v>
@@ -3576,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J65" s="2">
         <v>70</v>
@@ -3600,10 +3600,10 @@
         <v>4</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="D66" s="2">
         <v>12</v>
@@ -3621,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J66" s="2">
         <v>40</v>
@@ -3645,10 +3645,10 @@
         <v>4</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="D67" s="2">
         <v>14</v>
@@ -3666,7 +3666,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J67" s="2">
         <v>55</v>
@@ -3690,10 +3690,10 @@
         <v>4</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="D68" s="2">
         <v>11</v>
@@ -3711,7 +3711,7 @@
         <v>2</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J68" s="2">
         <v>55</v>
@@ -3735,10 +3735,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="D69" s="2">
         <v>6</v>
@@ -3756,7 +3756,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J69" s="2">
         <v>45</v>
@@ -3780,10 +3780,10 @@
         <v>4</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="D70" s="2">
         <v>7</v>
@@ -3801,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J70" s="2">
         <v>50</v>
@@ -3825,10 +3825,10 @@
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="D71" s="2">
         <v>12</v>
@@ -3846,7 +3846,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J71" s="2">
         <v>50</v>
@@ -3870,10 +3870,10 @@
         <v>4</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="D72" s="2">
         <v>8</v>
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J72" s="2">
         <v>60</v>
@@ -3915,10 +3915,10 @@
         <v>4</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D73" s="2">
         <v>15</v>
@@ -3936,7 +3936,7 @@
         <v>2</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J73" s="2">
         <v>55</v>
@@ -3960,10 +3960,10 @@
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="D74" s="2">
         <v>8</v>
@@ -3981,7 +3981,7 @@
         <v>2</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J74" s="2">
         <v>70</v>
@@ -4005,10 +4005,10 @@
         <v>4</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="D75" s="2">
         <v>10</v>
@@ -4026,7 +4026,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J75" s="2">
         <v>25</v>
@@ -4050,10 +4050,10 @@
         <v>4</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="D76" s="2">
         <v>6</v>
@@ -4071,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J76" s="2">
         <v>100</v>
@@ -4095,10 +4095,10 @@
         <v>4</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D77" s="2">
         <v>6</v>
@@ -4116,7 +4116,7 @@
         <v>2</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J77" s="2">
         <v>80</v>
@@ -4140,10 +4140,10 @@
         <v>4</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="D78" s="2">
         <v>8</v>
@@ -4161,7 +4161,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J78" s="2">
         <v>50</v>
@@ -4185,10 +4185,10 @@
         <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="D79" s="2">
         <v>13</v>
@@ -4206,7 +4206,7 @@
         <v>2</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J79" s="2">
         <v>75</v>
@@ -4230,10 +4230,10 @@
         <v>4</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D80" s="2">
         <v>5</v>
@@ -4251,7 +4251,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J80" s="2">
         <v>60</v>
@@ -4275,10 +4275,10 @@
         <v>4</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="D81" s="2">
         <v>4</v>
@@ -4296,7 +4296,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J81" s="2">
         <v>50</v>

</xml_diff>